<commit_message>
Actualziacion 16 de marzo 2017
</commit_message>
<xml_diff>
--- a/BITACORA INCIDENTES Y SOLICITUDES II.xlsx
+++ b/BITACORA INCIDENTES Y SOLICITUDES II.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="265">
   <si>
     <t>APLICACIÓN</t>
   </si>
@@ -878,9 +878,6 @@
     <t>15/03/2017  16:13:00 a. m.</t>
   </si>
   <si>
-    <t>reversion de pago montelibano</t>
-  </si>
-  <si>
     <t>CAPACITACION REQUERIDA</t>
   </si>
   <si>
@@ -918,6 +915,79 @@
   <si>
     <t>jesus vargas</t>
   </si>
+  <si>
+    <t>HACIENDA BARANOA</t>
+  </si>
+  <si>
+    <t>15/03/2017  18:13:00 a. m.</t>
+  </si>
+  <si>
+    <t>PAGOS SIN REGISTRAR</t>
+  </si>
+  <si>
+    <t>Buenas tardes
+Favor solicito revisar el estado de cuenta dela referencia catastral 010004840001000 a nombre de Pedro Blanco el contribuyente cancelo el pasado 13 de septiembre de 2016 las vigencias 2015 y 2016 y al acercarse a cancelar la vigencia 2017 se encuentra con la sorpresa que no aparecen aplicados los pagos de las respectivas vigencias, para lo cual envio recibos de caja del predial y la CRA.
+De igual forma revisando el reporte mensual del mes de septiembre de 2016 no aparece el número del recibo</t>
+  </si>
+  <si>
+    <t>AÑADICION DE ACTIVIDAD ICAT PARA LA ELABORACION DE DECLARACIONES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEÑORES: 
+COMERCIALIZADORA 
+CORDIAL SALUDO  
+SOLICITO ME COLABOREN INGRESANDO AL SISTEMA DE INDUSTRIA Y COMERCIO OTRO CÓDIGO DE UNA ACTIVIDAD FINANCIERA LLAMADA 
+ACTIVIDADES DE SERVICIO DE INFORMACION  LA TARIFA ES 10 X MIL.
+PARA PODER REGISTRAR  AL CONTRIBUYENTE 
+GRACIAS POR LA COLABORACION
+ATT </t>
+  </si>
+  <si>
+    <t>BUSCAR AUDITORIA DE PAGOS APLICADOS EN EL SISTEMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cordial saludo,
+Solicitamos la información de quien fue el funcionario responsable de aplicar el pago del recibo de estampillas contrato:
+Imágenes integradas 1
+Que aparece reportado en Swit con fecha 20-01-17.
+Igualmente necesitamos saber la información de la aplicación del recibo de maquinaria verde:
+Imágenes integradas 2
+Que aparece reportado en Swit con fecha 25-01-17.
+Favor informarnos de manera Urgente, ya que se está entregando informes a entes de control. Muchas Gracias.
+</t>
+  </si>
+  <si>
+    <t>CORRECION DE REVISORES Y RESPONSABLES FISCALES EN NOTAS CREDITO</t>
+  </si>
+  <si>
+    <t>Cordial saludo,
+Solicitamos por favor se corrija los nombres de las NOTAS CREDITO, ya que aparece el nombre del Tesorero del año anterior.
+Imágenes integradas 1
+Sugerimos se deje el cuadro en blanco como aparece actualmente en las NOTAS DEBITO.
+Imágenes integradas 2
+Favor revisar, muchas gracias.</t>
+  </si>
+  <si>
+    <t>revesion de pago montelibano</t>
+  </si>
+  <si>
+    <t>POLO NUEVO</t>
+  </si>
+  <si>
+    <t>Mariela Cervantes</t>
+  </si>
+  <si>
+    <t>16/03/2017  18:13:00 a. m.</t>
+  </si>
+  <si>
+    <t>Les solicito el favor de ayudarme para que el valor de los recibos 18 y 71 queden en cero pesos, debido a que alguien introdujo el nombre le Secretario de Hacienda y lo liquidaron un valor de $206.000 y el recibo No. 71 a nombre de la señora LADY JOHANA PIZARRO, es debido a que error involuntario lo liquide tres veces, como ustedes pueden apreciar en la planilla enviada, y estos valores están sumando a los ingresos. y estos valores no son verdad porque no están consignados en banco. 
+Agradezco su valiosa colaboración
+MARIELA CERVANTES
+Auxiliar Administrativo</t>
+  </si>
+  <si>
+    <t>REVERSION DE PAGOS POLO NUEVO</t>
+  </si>
 </sst>
 </file>
 
@@ -927,7 +997,7 @@
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-m\-yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1161,6 +1231,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1486,7 +1563,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="210">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1929,12 +2006,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2084,6 +2155,19 @@
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2490,11 +2574,11 @@
   <sheetPr codeName="Hoja1" filterMode="1"/>
   <dimension ref="A1:AM323"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomRight" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,25 +2703,25 @@
       <c r="B3" s="46"/>
       <c r="C3" s="20"/>
       <c r="D3" s="68"/>
-      <c r="E3" s="154" t="s">
+      <c r="E3" s="205" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="155"/>
-      <c r="J3" s="155"/>
-      <c r="K3" s="155"/>
-      <c r="L3" s="155"/>
-      <c r="M3" s="155"/>
-      <c r="N3" s="155"/>
-      <c r="O3" s="155"/>
-      <c r="P3" s="155"/>
-      <c r="Q3" s="155"/>
-      <c r="R3" s="155"/>
-      <c r="S3" s="155"/>
-      <c r="T3" s="155"/>
-      <c r="U3" s="155"/>
+      <c r="F3" s="206"/>
+      <c r="G3" s="206"/>
+      <c r="H3" s="206"/>
+      <c r="I3" s="206"/>
+      <c r="J3" s="206"/>
+      <c r="K3" s="206"/>
+      <c r="L3" s="206"/>
+      <c r="M3" s="206"/>
+      <c r="N3" s="206"/>
+      <c r="O3" s="206"/>
+      <c r="P3" s="206"/>
+      <c r="Q3" s="206"/>
+      <c r="R3" s="206"/>
+      <c r="S3" s="206"/>
+      <c r="T3" s="206"/>
+      <c r="U3" s="206"/>
       <c r="V3" s="11"/>
       <c r="W3" s="11"/>
       <c r="X3" s="11"/>
@@ -2664,23 +2748,23 @@
       <c r="B4" s="46"/>
       <c r="C4" s="20"/>
       <c r="D4" s="68"/>
-      <c r="E4" s="154"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="155"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
-      <c r="K4" s="155"/>
-      <c r="L4" s="155"/>
-      <c r="M4" s="155"/>
-      <c r="N4" s="155"/>
-      <c r="O4" s="155"/>
-      <c r="P4" s="155"/>
-      <c r="Q4" s="155"/>
-      <c r="R4" s="155"/>
-      <c r="S4" s="155"/>
-      <c r="T4" s="155"/>
-      <c r="U4" s="155"/>
+      <c r="E4" s="205"/>
+      <c r="F4" s="206"/>
+      <c r="G4" s="206"/>
+      <c r="H4" s="206"/>
+      <c r="I4" s="206"/>
+      <c r="J4" s="206"/>
+      <c r="K4" s="206"/>
+      <c r="L4" s="206"/>
+      <c r="M4" s="206"/>
+      <c r="N4" s="206"/>
+      <c r="O4" s="206"/>
+      <c r="P4" s="206"/>
+      <c r="Q4" s="206"/>
+      <c r="R4" s="206"/>
+      <c r="S4" s="206"/>
+      <c r="T4" s="206"/>
+      <c r="U4" s="206"/>
       <c r="V4" s="11"/>
       <c r="W4" s="11"/>
       <c r="X4" s="11"/>
@@ -3067,65 +3151,65 @@
       </c>
       <c r="Z10" s="73"/>
     </row>
-    <row r="11" spans="1:39" s="175" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="156" t="s">
+    <row r="11" spans="1:39" s="173" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="154" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="157">
+      <c r="B11" s="155">
         <v>361</v>
       </c>
-      <c r="C11" s="158" t="s">
+      <c r="C11" s="156" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="159" t="s">
+      <c r="D11" s="157" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="160" t="s">
+      <c r="E11" s="158" t="s">
         <v>114</v>
       </c>
-      <c r="F11" s="161" t="s">
+      <c r="F11" s="159" t="s">
         <v>133</v>
       </c>
-      <c r="G11" s="162" t="s">
+      <c r="G11" s="160" t="s">
         <v>105</v>
       </c>
-      <c r="H11" s="163" t="s">
+      <c r="H11" s="161" t="s">
         <v>134</v>
       </c>
-      <c r="I11" s="164" t="s">
+      <c r="I11" s="162" t="s">
         <v>107</v>
       </c>
-      <c r="J11" s="165"/>
-      <c r="K11" s="165" t="s">
+      <c r="J11" s="163"/>
+      <c r="K11" s="163" t="s">
         <v>135</v>
       </c>
-      <c r="L11" s="165"/>
-      <c r="M11" s="164" t="s">
+      <c r="L11" s="163"/>
+      <c r="M11" s="162" t="s">
         <v>128</v>
       </c>
-      <c r="N11" s="166" t="s">
+      <c r="N11" s="164" t="s">
         <v>136</v>
       </c>
-      <c r="O11" s="164" t="s">
+      <c r="O11" s="162" t="s">
         <v>36</v>
       </c>
-      <c r="P11" s="164" t="s">
+      <c r="P11" s="162" t="s">
         <v>36</v>
       </c>
-      <c r="Q11" s="164"/>
-      <c r="R11" s="167"/>
-      <c r="S11" s="168" t="s">
+      <c r="Q11" s="162"/>
+      <c r="R11" s="165"/>
+      <c r="S11" s="166" t="s">
         <v>110</v>
       </c>
-      <c r="T11" s="161"/>
-      <c r="U11" s="169"/>
-      <c r="V11" s="170" t="s">
+      <c r="T11" s="159"/>
+      <c r="U11" s="167"/>
+      <c r="V11" s="168" t="s">
         <v>141</v>
       </c>
-      <c r="W11" s="171"/>
-      <c r="X11" s="172"/>
-      <c r="Y11" s="173"/>
-      <c r="Z11" s="174"/>
+      <c r="W11" s="169"/>
+      <c r="X11" s="170"/>
+      <c r="Y11" s="171"/>
+      <c r="Z11" s="172"/>
     </row>
     <row r="12" spans="1:39" s="27" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
@@ -4093,63 +4177,63 @@
       <c r="Y27" s="34"/>
       <c r="Z27" s="73"/>
     </row>
-    <row r="28" spans="1:26" s="175" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="156" t="s">
+    <row r="28" spans="1:26" s="173" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="176">
+      <c r="B28" s="174">
         <v>364</v>
       </c>
-      <c r="C28" s="177" t="s">
+      <c r="C28" s="175" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="178" t="s">
+      <c r="D28" s="176" t="s">
         <v>113</v>
       </c>
-      <c r="E28" s="179" t="s">
+      <c r="E28" s="177" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="180">
+      <c r="F28" s="178">
         <v>42807.625</v>
       </c>
-      <c r="G28" s="181" t="s">
+      <c r="G28" s="179" t="s">
         <v>105</v>
       </c>
-      <c r="H28" s="182" t="s">
+      <c r="H28" s="180" t="s">
         <v>211</v>
       </c>
-      <c r="I28" s="177" t="s">
+      <c r="I28" s="175" t="s">
         <v>212</v>
       </c>
-      <c r="J28" s="183"/>
-      <c r="K28" s="183" t="s">
+      <c r="J28" s="181"/>
+      <c r="K28" s="181" t="s">
         <v>213</v>
       </c>
-      <c r="L28" s="183"/>
-      <c r="M28" s="177" t="s">
+      <c r="L28" s="181"/>
+      <c r="M28" s="175" t="s">
         <v>146</v>
       </c>
-      <c r="N28" s="183"/>
-      <c r="O28" s="177" t="s">
+      <c r="N28" s="181"/>
+      <c r="O28" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="P28" s="177" t="s">
+      <c r="P28" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="Q28" s="177"/>
-      <c r="R28" s="180"/>
-      <c r="S28" s="184" t="s">
+      <c r="Q28" s="175"/>
+      <c r="R28" s="178"/>
+      <c r="S28" s="182" t="s">
         <v>110</v>
       </c>
-      <c r="T28" s="180"/>
-      <c r="U28" s="185"/>
-      <c r="V28" s="186" t="s">
+      <c r="T28" s="178"/>
+      <c r="U28" s="183"/>
+      <c r="V28" s="184" t="s">
         <v>173</v>
       </c>
-      <c r="W28" s="187"/>
-      <c r="X28" s="188"/>
-      <c r="Y28" s="189"/>
-      <c r="Z28" s="174"/>
+      <c r="W28" s="185"/>
+      <c r="X28" s="186"/>
+      <c r="Y28" s="187"/>
+      <c r="Z28" s="172"/>
     </row>
     <row r="29" spans="1:26" s="27" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
@@ -4381,63 +4465,63 @@
       <c r="Y32" s="34"/>
       <c r="Z32" s="73"/>
     </row>
-    <row r="33" spans="1:26" s="175" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="156" t="s">
+    <row r="33" spans="1:26" s="173" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="154" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="190" t="s">
+      <c r="B33" s="188" t="s">
         <v>226</v>
       </c>
-      <c r="C33" s="177" t="s">
+      <c r="C33" s="175" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="178" t="s">
+      <c r="D33" s="176" t="s">
         <v>113</v>
       </c>
-      <c r="E33" s="179" t="s">
+      <c r="E33" s="177" t="s">
         <v>114</v>
       </c>
-      <c r="F33" s="180">
+      <c r="F33" s="178">
         <v>42809.342361111114</v>
       </c>
-      <c r="G33" s="181" t="s">
+      <c r="G33" s="179" t="s">
         <v>105</v>
       </c>
-      <c r="H33" s="182" t="s">
+      <c r="H33" s="180" t="s">
         <v>227</v>
       </c>
-      <c r="I33" s="177" t="s">
+      <c r="I33" s="175" t="s">
         <v>125</v>
       </c>
-      <c r="J33" s="183"/>
-      <c r="K33" s="183" t="s">
+      <c r="J33" s="181"/>
+      <c r="K33" s="181" t="s">
         <v>228</v>
       </c>
-      <c r="L33" s="183"/>
-      <c r="M33" s="177" t="s">
+      <c r="L33" s="181"/>
+      <c r="M33" s="175" t="s">
         <v>217</v>
       </c>
-      <c r="N33" s="183"/>
-      <c r="O33" s="177" t="s">
+      <c r="N33" s="181"/>
+      <c r="O33" s="175" t="s">
         <v>24</v>
       </c>
-      <c r="P33" s="177" t="s">
+      <c r="P33" s="175" t="s">
         <v>24</v>
       </c>
-      <c r="Q33" s="177"/>
-      <c r="R33" s="180"/>
-      <c r="S33" s="184" t="s">
+      <c r="Q33" s="175"/>
+      <c r="R33" s="178"/>
+      <c r="S33" s="182" t="s">
         <v>217</v>
       </c>
-      <c r="T33" s="180"/>
-      <c r="U33" s="185"/>
-      <c r="V33" s="187" t="s">
+      <c r="T33" s="178"/>
+      <c r="U33" s="183"/>
+      <c r="V33" s="185" t="s">
         <v>25</v>
       </c>
-      <c r="W33" s="187"/>
-      <c r="X33" s="188"/>
-      <c r="Y33" s="189"/>
-      <c r="Z33" s="174"/>
+      <c r="W33" s="185"/>
+      <c r="X33" s="186"/>
+      <c r="Y33" s="187"/>
+      <c r="Z33" s="172"/>
     </row>
     <row r="34" spans="1:26" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
@@ -4553,65 +4637,65 @@
       <c r="Y35" s="34"/>
       <c r="Z35" s="73"/>
     </row>
-    <row r="36" spans="1:26" s="206" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="191" t="s">
+    <row r="36" spans="1:26" s="204" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="189" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="192" t="s">
+      <c r="B36" s="190" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="193" t="s">
+      <c r="C36" s="191" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="194" t="s">
+      <c r="D36" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="E36" s="195" t="s">
+      <c r="E36" s="193" t="s">
         <v>235</v>
       </c>
-      <c r="F36" s="196" t="s">
+      <c r="F36" s="194" t="s">
         <v>236</v>
       </c>
-      <c r="G36" s="197" t="s">
+      <c r="G36" s="195" t="s">
         <v>105</v>
       </c>
-      <c r="H36" s="198" t="s">
+      <c r="H36" s="196" t="s">
         <v>237</v>
       </c>
-      <c r="I36" s="193" t="s">
+      <c r="I36" s="191" t="s">
         <v>238</v>
       </c>
-      <c r="J36" s="199"/>
-      <c r="K36" s="199" t="s">
+      <c r="J36" s="197"/>
+      <c r="K36" s="197" t="s">
         <v>239</v>
       </c>
-      <c r="L36" s="199"/>
-      <c r="M36" s="193" t="s">
+      <c r="L36" s="197"/>
+      <c r="M36" s="191" t="s">
         <v>120</v>
       </c>
-      <c r="N36" s="199"/>
-      <c r="O36" s="193" t="s">
+      <c r="N36" s="197"/>
+      <c r="O36" s="191" t="s">
         <v>153</v>
       </c>
-      <c r="P36" s="193" t="s">
+      <c r="P36" s="191" t="s">
         <v>36</v>
       </c>
-      <c r="Q36" s="193"/>
-      <c r="R36" s="196"/>
-      <c r="S36" s="200" t="s">
+      <c r="Q36" s="191"/>
+      <c r="R36" s="194"/>
+      <c r="S36" s="198" t="s">
         <v>110</v>
       </c>
-      <c r="T36" s="196"/>
-      <c r="U36" s="201"/>
-      <c r="V36" s="202" t="s">
+      <c r="T36" s="194"/>
+      <c r="U36" s="199"/>
+      <c r="V36" s="200" t="s">
         <v>173</v>
       </c>
-      <c r="W36" s="202"/>
-      <c r="X36" s="203"/>
-      <c r="Y36" s="204"/>
-      <c r="Z36" s="205"/>
-    </row>
-    <row r="37" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W36" s="200"/>
+      <c r="X36" s="201"/>
+      <c r="Y36" s="202"/>
+      <c r="Z36" s="203"/>
+    </row>
+    <row r="37" spans="1:26" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
         <v>73</v>
       </c>
@@ -4634,7 +4718,7 @@
         <v>105</v>
       </c>
       <c r="H37" s="65" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="I37" s="30" t="s">
         <v>125</v>
@@ -4660,7 +4744,7 @@
       <c r="T37" s="35"/>
       <c r="U37" s="36"/>
       <c r="V37" s="32" t="s">
-        <v>173</v>
+        <v>31</v>
       </c>
       <c r="W37" s="32"/>
       <c r="X37" s="33"/>
@@ -4690,14 +4774,14 @@
         <v>105</v>
       </c>
       <c r="H38" s="65" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I38" s="30" t="s">
         <v>125</v>
       </c>
       <c r="J38" s="38"/>
       <c r="K38" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L38" s="38"/>
       <c r="M38" s="30" t="s">
@@ -4725,7 +4809,7 @@
       <c r="Y38" s="34"/>
       <c r="Z38" s="73"/>
     </row>
-    <row r="39" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="s">
         <v>75</v>
       </c>
@@ -4748,14 +4832,14 @@
         <v>105</v>
       </c>
       <c r="H39" s="65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I39" s="30" t="s">
         <v>125</v>
       </c>
       <c r="J39" s="38"/>
       <c r="K39" s="38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L39" s="38"/>
       <c r="M39" s="30" t="s">
@@ -4776,7 +4860,7 @@
       <c r="T39" s="35"/>
       <c r="U39" s="36"/>
       <c r="V39" s="32" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="W39" s="32"/>
       <c r="X39" s="33"/>
@@ -4797,16 +4881,16 @@
         <v>103</v>
       </c>
       <c r="E40" s="150" t="s">
+        <v>245</v>
+      </c>
+      <c r="F40" s="35" t="s">
         <v>246</v>
-      </c>
-      <c r="F40" s="35" t="s">
-        <v>247</v>
       </c>
       <c r="G40" s="52" t="s">
         <v>105</v>
       </c>
       <c r="H40" s="65" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I40" s="30" t="s">
         <v>125</v>
@@ -4827,7 +4911,7 @@
       <c r="Q40" s="30"/>
       <c r="R40" s="31"/>
       <c r="S40" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="T40" s="35"/>
       <c r="U40" s="36"/>
@@ -4839,151 +4923,291 @@
       <c r="Y40" s="34"/>
       <c r="Z40" s="73"/>
     </row>
-    <row r="41" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
+    <row r="41" spans="1:26" s="204" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="189" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="49"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="150"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="65"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="38"/>
-      <c r="L41" s="38"/>
-      <c r="M41" s="30"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="31"/>
-      <c r="S41" s="29"/>
-      <c r="T41" s="35"/>
-      <c r="U41" s="36"/>
-      <c r="V41" s="32"/>
-      <c r="W41" s="32"/>
-      <c r="X41" s="33"/>
-      <c r="Y41" s="34"/>
-      <c r="Z41" s="73"/>
-    </row>
-    <row r="42" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="44" t="s">
+      <c r="B41" s="190" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="191" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="207" t="s">
+        <v>230</v>
+      </c>
+      <c r="E41" s="193" t="s">
+        <v>249</v>
+      </c>
+      <c r="F41" s="194" t="s">
+        <v>250</v>
+      </c>
+      <c r="G41" s="195" t="s">
+        <v>105</v>
+      </c>
+      <c r="H41" s="196" t="s">
+        <v>251</v>
+      </c>
+      <c r="I41" s="191" t="s">
+        <v>125</v>
+      </c>
+      <c r="J41" s="197"/>
+      <c r="K41" s="197" t="s">
+        <v>252</v>
+      </c>
+      <c r="L41" s="197"/>
+      <c r="M41" s="191" t="s">
+        <v>195</v>
+      </c>
+      <c r="N41" s="197"/>
+      <c r="O41" s="191" t="s">
+        <v>153</v>
+      </c>
+      <c r="P41" s="191" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q41" s="191"/>
+      <c r="R41" s="208"/>
+      <c r="S41" s="198" t="s">
+        <v>110</v>
+      </c>
+      <c r="T41" s="194"/>
+      <c r="U41" s="199"/>
+      <c r="V41" t="s">
+        <v>31</v>
+      </c>
+      <c r="W41" s="200"/>
+      <c r="X41" s="201"/>
+      <c r="Y41" s="202"/>
+      <c r="Z41" s="203"/>
+    </row>
+    <row r="42" spans="1:26" s="204" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="189" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="49"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="150"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="38"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="38"/>
-      <c r="M42" s="30"/>
-      <c r="N42" s="38"/>
-      <c r="O42" s="30"/>
-      <c r="P42" s="30"/>
-      <c r="Q42" s="30"/>
-      <c r="R42" s="31"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="35"/>
-      <c r="U42" s="36"/>
-      <c r="V42" s="32"/>
-      <c r="W42" s="32"/>
-      <c r="X42" s="33"/>
-      <c r="Y42" s="34"/>
-      <c r="Z42" s="73"/>
-    </row>
-    <row r="43" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="190" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="191" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" s="207" t="s">
+        <v>234</v>
+      </c>
+      <c r="E42" s="193" t="s">
+        <v>235</v>
+      </c>
+      <c r="F42" s="194" t="s">
+        <v>250</v>
+      </c>
+      <c r="G42" s="195" t="s">
+        <v>105</v>
+      </c>
+      <c r="H42" s="196" t="s">
+        <v>253</v>
+      </c>
+      <c r="I42" s="191" t="s">
+        <v>125</v>
+      </c>
+      <c r="J42" s="197"/>
+      <c r="K42" s="197" t="s">
+        <v>254</v>
+      </c>
+      <c r="L42" s="197"/>
+      <c r="M42" s="191" t="s">
+        <v>183</v>
+      </c>
+      <c r="N42" s="197"/>
+      <c r="O42" s="191" t="s">
+        <v>153</v>
+      </c>
+      <c r="P42" s="191" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q42" s="191"/>
+      <c r="R42" s="208"/>
+      <c r="S42" s="198" t="s">
+        <v>110</v>
+      </c>
+      <c r="T42" s="194"/>
+      <c r="U42" s="199"/>
+      <c r="V42" s="200" t="s">
+        <v>173</v>
+      </c>
+      <c r="W42" s="200"/>
+      <c r="X42" s="201"/>
+      <c r="Y42" s="202"/>
+      <c r="Z42" s="203"/>
+    </row>
+    <row r="43" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="49"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="90"/>
-      <c r="E43" s="150"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="65"/>
-      <c r="I43" s="30"/>
+      <c r="B43" s="49">
+        <v>367</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" s="90" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" s="150" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="35">
+        <v>42810.300694444442</v>
+      </c>
+      <c r="G43" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="H43" s="65" t="s">
+        <v>255</v>
+      </c>
+      <c r="I43" s="30" t="s">
+        <v>125</v>
+      </c>
       <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
+      <c r="K43" s="38" t="s">
+        <v>256</v>
+      </c>
       <c r="L43" s="38"/>
-      <c r="M43" s="30"/>
+      <c r="M43" s="30" t="s">
+        <v>172</v>
+      </c>
       <c r="N43" s="38"/>
-      <c r="O43" s="30"/>
-      <c r="P43" s="30"/>
+      <c r="O43" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="P43" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="Q43" s="30"/>
       <c r="R43" s="31"/>
-      <c r="S43" s="29"/>
+      <c r="S43" s="29" t="s">
+        <v>110</v>
+      </c>
       <c r="T43" s="35"/>
       <c r="U43" s="36"/>
-      <c r="V43" s="32"/>
+      <c r="V43" s="32" t="s">
+        <v>31</v>
+      </c>
       <c r="W43" s="32"/>
       <c r="X43" s="33"/>
       <c r="Y43" s="34"/>
       <c r="Z43" s="73"/>
     </row>
-    <row r="44" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" s="27" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="49"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="90"/>
-      <c r="E44" s="150"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="65"/>
-      <c r="I44" s="30"/>
+      <c r="B44" s="49">
+        <v>368</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" s="90" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" s="150" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="35">
+        <v>42810.356249999997</v>
+      </c>
+      <c r="G44" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="H44" s="65" t="s">
+        <v>257</v>
+      </c>
+      <c r="I44" s="30" t="s">
+        <v>125</v>
+      </c>
       <c r="J44" s="38"/>
-      <c r="K44" s="38"/>
+      <c r="K44" s="38" t="s">
+        <v>258</v>
+      </c>
       <c r="L44" s="38"/>
-      <c r="M44" s="30"/>
+      <c r="M44" s="30" t="s">
+        <v>183</v>
+      </c>
       <c r="N44" s="38"/>
-      <c r="O44" s="30"/>
-      <c r="P44" s="30"/>
+      <c r="O44" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="P44" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="Q44" s="30"/>
       <c r="R44" s="35"/>
-      <c r="S44" s="29"/>
+      <c r="S44" s="29" t="s">
+        <v>110</v>
+      </c>
       <c r="T44" s="35"/>
       <c r="U44" s="36"/>
-      <c r="V44" s="32"/>
+      <c r="V44" s="32" t="s">
+        <v>31</v>
+      </c>
       <c r="W44" s="32"/>
       <c r="X44" s="33"/>
       <c r="Y44" s="34"/>
       <c r="Z44" s="73"/>
     </row>
-    <row r="45" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="49"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="76"/>
-      <c r="E45" s="150"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="65"/>
-      <c r="I45" s="30"/>
+      <c r="B45" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" s="76" t="s">
+        <v>260</v>
+      </c>
+      <c r="E45" s="209" t="s">
+        <v>261</v>
+      </c>
+      <c r="F45" s="194" t="s">
+        <v>262</v>
+      </c>
+      <c r="G45" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="H45" s="65" t="s">
+        <v>264</v>
+      </c>
+      <c r="I45" s="30" t="s">
+        <v>125</v>
+      </c>
       <c r="J45" s="38"/>
-      <c r="K45" s="38"/>
+      <c r="K45" s="38" t="s">
+        <v>263</v>
+      </c>
       <c r="L45" s="38"/>
-      <c r="M45" s="30"/>
+      <c r="M45" s="30" t="s">
+        <v>183</v>
+      </c>
       <c r="N45" s="38"/>
-      <c r="O45" s="30"/>
-      <c r="P45" s="30"/>
+      <c r="O45" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="P45" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="Q45" s="30"/>
       <c r="R45" s="31"/>
-      <c r="S45" s="29"/>
+      <c r="S45" s="29" t="s">
+        <v>110</v>
+      </c>
       <c r="T45" s="35"/>
       <c r="U45" s="36"/>
-      <c r="V45" s="56"/>
+      <c r="V45" s="56" t="s">
+        <v>173</v>
+      </c>
       <c r="W45" s="32"/>
       <c r="X45" s="33"/>
       <c r="Y45" s="34"/>
@@ -11756,7 +11980,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ACTUALIZACION DE BITACORA 18/03/17
</commit_message>
<xml_diff>
--- a/BITACORA INCIDENTES Y SOLICITUDES II.xlsx
+++ b/BITACORA INCIDENTES Y SOLICITUDES II.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="272">
   <si>
     <t>APLICACIÓN</t>
   </si>
@@ -1018,6 +1018,19 @@
 --
 Secretaría de Hacienda
 Alcaldía Municipal de Ipiales</t>
+  </si>
+  <si>
+    <t>VERIFICAR CUAL CONSECUTIVO SE MOSTRARA EN EL PANEL Y EN EL FORMULARIO</t>
+  </si>
+  <si>
+    <t>Cordial saludo,
+Con respecto a las solicitudes mencionadas se realizó el proceso descrito, pero al momento de imprimir copia de las declaraciones para anexarlas al respectivo reporte, nos percatamos que el sistema le asigno otro número a la declaración diferente al que se ingresó al momento de sistematizar la declaración (imagen adjunta). Por tal razón solicitamos nos colaboren con el cambio del numero de la declaración que el sistema esta asignando y se deje el numero correcto que debe tener la declaración.
+Las declaraciones que se sistematizaron son sus respectivos contribuyentes son:
+declaracion                           Nit                        aparece al imprimir
+16020110002609                   36992717               17020110001000
+16020110001617                   13006005               17020110001686
+16020110001549                   27167805               17020110001771
+16020110001542                   1085932129            17020110001772</t>
   </si>
 </sst>
 </file>
@@ -2602,14 +2615,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1" filterMode="1"/>
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AM323"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="T8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="G55" sqref="G55"/>
+      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,7 +2991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:39" s="27" customFormat="1" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" s="27" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="116" t="s">
         <v>44</v>
       </c>
@@ -3046,7 +3059,7 @@
       </c>
       <c r="Z8" s="73"/>
     </row>
-    <row r="9" spans="1:39" s="28" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" s="28" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
         <v>45</v>
       </c>
@@ -3114,7 +3127,7 @@
       </c>
       <c r="Z9" s="73"/>
     </row>
-    <row r="10" spans="1:39" s="27" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
         <v>46</v>
       </c>
@@ -3182,7 +3195,7 @@
       </c>
       <c r="Z10" s="73"/>
     </row>
-    <row r="11" spans="1:39" s="173" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" s="173" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="154" t="s">
         <v>47</v>
       </c>
@@ -3242,7 +3255,7 @@
       <c r="Y11" s="171"/>
       <c r="Z11" s="172"/>
     </row>
-    <row r="12" spans="1:39" s="27" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
         <v>48</v>
       </c>
@@ -3310,7 +3323,7 @@
       </c>
       <c r="Z12" s="73"/>
     </row>
-    <row r="13" spans="1:39" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>49</v>
       </c>
@@ -3376,7 +3389,7 @@
       </c>
       <c r="Z13" s="73"/>
     </row>
-    <row r="14" spans="1:39" s="27" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>50</v>
       </c>
@@ -3440,7 +3453,7 @@
       </c>
       <c r="Z14" s="73"/>
     </row>
-    <row r="15" spans="1:39" s="27" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>51</v>
       </c>
@@ -3502,7 +3515,7 @@
       <c r="Y15" s="34"/>
       <c r="Z15" s="73"/>
     </row>
-    <row r="16" spans="1:39" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="44" t="s">
         <v>52</v>
       </c>
@@ -3562,7 +3575,7 @@
       <c r="Y16" s="34"/>
       <c r="Z16" s="73"/>
     </row>
-    <row r="17" spans="1:26" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="44" t="s">
         <v>53</v>
       </c>
@@ -3626,7 +3639,7 @@
       </c>
       <c r="Z17" s="73"/>
     </row>
-    <row r="18" spans="1:26" s="27" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" s="27" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
         <v>54</v>
       </c>
@@ -3684,7 +3697,7 @@
       <c r="Y18" s="34"/>
       <c r="Z18" s="73"/>
     </row>
-    <row r="19" spans="1:26" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
         <v>55</v>
       </c>
@@ -3732,7 +3745,7 @@
       <c r="Y19" s="34"/>
       <c r="Z19" s="73"/>
     </row>
-    <row r="20" spans="1:26" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="44" t="s">
         <v>56</v>
       </c>
@@ -3790,7 +3803,7 @@
       <c r="Y20" s="34"/>
       <c r="Z20" s="73"/>
     </row>
-    <row r="21" spans="1:26" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="44" t="s">
         <v>57</v>
       </c>
@@ -3850,7 +3863,7 @@
       <c r="Y21" s="34"/>
       <c r="Z21" s="73"/>
     </row>
-    <row r="22" spans="1:26" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
         <v>58</v>
       </c>
@@ -3910,7 +3923,7 @@
       <c r="Y22" s="34"/>
       <c r="Z22" s="73"/>
     </row>
-    <row r="23" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="s">
         <v>59</v>
       </c>
@@ -3972,7 +3985,7 @@
       <c r="Y23" s="34"/>
       <c r="Z23" s="73"/>
     </row>
-    <row r="24" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
         <v>60</v>
       </c>
@@ -4034,7 +4047,7 @@
       <c r="Y24" s="34"/>
       <c r="Z24" s="73"/>
     </row>
-    <row r="25" spans="1:26" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="s">
         <v>61</v>
       </c>
@@ -4088,7 +4101,7 @@
       <c r="Y25" s="34"/>
       <c r="Z25" s="73"/>
     </row>
-    <row r="26" spans="1:26" s="27" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" s="27" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="s">
         <v>62</v>
       </c>
@@ -4150,7 +4163,7 @@
       <c r="Y26" s="34"/>
       <c r="Z26" s="73"/>
     </row>
-    <row r="27" spans="1:26" s="27" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
         <v>63</v>
       </c>
@@ -4266,7 +4279,7 @@
       <c r="Y28" s="187"/>
       <c r="Z28" s="172"/>
     </row>
-    <row r="29" spans="1:26" s="27" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
         <v>65</v>
       </c>
@@ -4324,7 +4337,7 @@
       <c r="Y29" s="34"/>
       <c r="Z29" s="73"/>
     </row>
-    <row r="30" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
         <v>66</v>
       </c>
@@ -4380,7 +4393,7 @@
       <c r="Y30" s="34"/>
       <c r="Z30" s="73"/>
     </row>
-    <row r="31" spans="1:26" s="27" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" s="27" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
         <v>67</v>
       </c>
@@ -4438,7 +4451,7 @@
       <c r="Y31" s="34"/>
       <c r="Z31" s="73"/>
     </row>
-    <row r="32" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="s">
         <v>68</v>
       </c>
@@ -4554,7 +4567,7 @@
       <c r="Y33" s="187"/>
       <c r="Z33" s="172"/>
     </row>
-    <row r="34" spans="1:26" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
         <v>70</v>
       </c>
@@ -4610,7 +4623,7 @@
       <c r="Y34" s="34"/>
       <c r="Z34" s="73"/>
     </row>
-    <row r="35" spans="1:26" s="27" customFormat="1" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" s="27" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
         <v>71</v>
       </c>
@@ -4668,7 +4681,7 @@
       <c r="Y35" s="34"/>
       <c r="Z35" s="73"/>
     </row>
-    <row r="36" spans="1:26" s="204" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" s="204" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="189" t="s">
         <v>72</v>
       </c>
@@ -4726,7 +4739,7 @@
       <c r="Y36" s="202"/>
       <c r="Z36" s="203"/>
     </row>
-    <row r="37" spans="1:26" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
         <v>73</v>
       </c>
@@ -4782,7 +4795,7 @@
       <c r="Y37" s="34"/>
       <c r="Z37" s="73"/>
     </row>
-    <row r="38" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="s">
         <v>74</v>
       </c>
@@ -4840,7 +4853,7 @@
       <c r="Y38" s="34"/>
       <c r="Z38" s="73"/>
     </row>
-    <row r="39" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="s">
         <v>75</v>
       </c>
@@ -4898,7 +4911,7 @@
       <c r="Y39" s="34"/>
       <c r="Z39" s="73"/>
     </row>
-    <row r="40" spans="1:26" s="27" customFormat="1" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" s="27" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="44" t="s">
         <v>76</v>
       </c>
@@ -4954,7 +4967,7 @@
       <c r="Y40" s="34"/>
       <c r="Z40" s="73"/>
     </row>
-    <row r="41" spans="1:26" s="204" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" s="204" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="189" t="s">
         <v>77</v>
       </c>
@@ -5062,15 +5075,15 @@
       </c>
       <c r="T42" s="194"/>
       <c r="U42" s="199"/>
-      <c r="V42" s="32" t="s">
-        <v>172</v>
+      <c r="V42" t="s">
+        <v>31</v>
       </c>
       <c r="W42" s="200"/>
       <c r="X42" s="201"/>
       <c r="Y42" s="202"/>
       <c r="Z42" s="203"/>
     </row>
-    <row r="43" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
         <v>79</v>
       </c>
@@ -5128,7 +5141,7 @@
       <c r="Y43" s="34"/>
       <c r="Z43" s="73"/>
     </row>
-    <row r="44" spans="1:26" s="27" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
         <v>80</v>
       </c>
@@ -5186,7 +5199,7 @@
       <c r="Y44" s="34"/>
       <c r="Z44" s="73"/>
     </row>
-    <row r="45" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="s">
         <v>81</v>
       </c>
@@ -5244,7 +5257,7 @@
       <c r="Y45" s="34"/>
       <c r="Z45" s="73"/>
     </row>
-    <row r="46" spans="1:26" s="27" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" s="27" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="s">
         <v>82</v>
       </c>
@@ -5302,7 +5315,7 @@
       <c r="Y46" s="34"/>
       <c r="Z46" s="73"/>
     </row>
-    <row r="47" spans="1:26" s="27" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
         <v>83</v>
       </c>
@@ -5418,31 +5431,59 @@
       <c r="Y48" s="34"/>
       <c r="Z48" s="73"/>
     </row>
-    <row r="49" spans="1:26" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" s="27" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="49"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="76"/>
-      <c r="E49" s="150"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="65"/>
-      <c r="I49" s="30"/>
+      <c r="B49" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="76" t="s">
+        <v>113</v>
+      </c>
+      <c r="E49" s="150" t="s">
+        <v>114</v>
+      </c>
+      <c r="F49" s="35">
+        <v>42812.436805555553</v>
+      </c>
+      <c r="G49" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="H49" s="65" t="s">
+        <v>270</v>
+      </c>
+      <c r="I49" s="30" t="s">
+        <v>125</v>
+      </c>
       <c r="J49" s="38"/>
-      <c r="K49" s="38"/>
+      <c r="K49" s="38" t="s">
+        <v>271</v>
+      </c>
       <c r="L49" s="38"/>
-      <c r="M49" s="30"/>
+      <c r="M49" s="30" t="s">
+        <v>110</v>
+      </c>
       <c r="N49" s="38"/>
-      <c r="O49" s="30"/>
-      <c r="P49" s="30"/>
+      <c r="O49" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="P49" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="Q49" s="30"/>
       <c r="R49" s="35"/>
-      <c r="S49" s="29"/>
+      <c r="S49" s="29" t="s">
+        <v>110</v>
+      </c>
       <c r="T49" s="35"/>
       <c r="U49" s="36"/>
-      <c r="V49" s="32"/>
+      <c r="V49" s="32" t="s">
+        <v>25</v>
+      </c>
       <c r="W49" s="32"/>
       <c r="X49" s="33"/>
       <c r="Y49" s="34"/>
@@ -12062,14 +12103,7 @@
       <c r="W323" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A7:AM125">
-    <filterColumn colId="21">
-      <filters blank="1">
-        <filter val="ESCALADO A FUNCIONAL"/>
-        <filter val="ESCALADO A SISTEMAS"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A7:AM125"/>
   <mergeCells count="1">
     <mergeCell ref="E3:U4"/>
   </mergeCells>
@@ -12094,7 +12128,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>